<commit_message>
Single function output now working with named areas
</commit_message>
<xml_diff>
--- a/examples/singlefunctionc.xlsx
+++ b/examples/singlefunctionc.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="input">Sheet1!$B$1</definedName>
+    <definedName name="inputs">Sheet1!$C$1:$F$1</definedName>
     <definedName name="output">Sheet1!$B$2</definedName>
+    <definedName name="outputs">Sheet1!$C$2:$F$2</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -35,10 +37,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,13 +79,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,23 +423,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>100</v>
       </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>30</v>
+      </c>
+      <c r="F1">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -421,9 +459,26 @@
         <f>EXP(-1/input)</f>
         <v>0.99004983374916811</v>
       </c>
+      <c r="C2">
+        <f>F2-10</f>
+        <v>-9.0246900879716669</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:F2" si="0">EXP(-1/D1)</f>
+        <v>0.95122942450071402</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>0.9672161004820059</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>0.97530991202833262</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Remove brackets when replacing formulae with their values
</commit_message>
<xml_diff>
--- a/examples/singlefunctionc.xlsx
+++ b/examples/singlefunctionc.xlsx
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Input</t>
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>Constant</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -456,8 +459,8 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>EXP(-1/input)</f>
-        <v>0.99004983374916811</v>
+        <f>EXP(-1/input)+(B3)</f>
+        <v>12.990049833749168</v>
       </c>
       <c r="C2">
         <f>F2-10</f>
@@ -474,6 +477,14 @@
       <c r="F2">
         <f t="shared" si="0"/>
         <v>0.97530991202833262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>